<commit_message>
house robber O(1) solution
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AB5C34-8B79-6343-9BDE-0491BA2DB32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC82F097-C169-984E-A0D0-62B75FB7D716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27680" yWindow="2360" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="172">
   <si>
     <t>Category</t>
   </si>
@@ -1291,6 +1291,50 @@
   </si>
   <si>
     <t>generating permutations. Or adding all the way up.</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def rob(self, nums: List[int]) -&gt; int:
+        def robHelp(i, result):
+            if i&gt;len(nums)-1:
+                return result
+            return max(robHelp(i+2, result+nums[i]),robHelp(i+1, result))
+        return robHelp(0,0)</t>
+  </si>
+  <si>
+    <t>House Robber </t>
+  </si>
+  <si>
+    <t>Good problem to understand</t>
+  </si>
+  <si>
+    <t>DP - O(1) solution
+class Solution:
+    def rob(self, nums: List[int]) -&gt; int:
+        #rob2 is previous house we robbed. rob1 is before that
+        rob1, rob2 = 0, 0
+        for n in nums:
+            temp = max(n + rob1, rob2)
+            rob1 = rob2
+            rob2 = temp
+        return rob2
+DP - O(n) solution:
+class Solution:
+    def rob(self, nums: List[int]) -&gt; int:
+        n=len(nums)
+        if n==0:
+            return 0
+        elif n==1:
+            return nums[0]
+        dp=[0]*n
+        dp[0]=nums[0]
+        dp[1]=max(nums[0],nums[1])
+        for i in range(2,n):
+            dp[i]=max(dp[i-1],nums[i]+dp[i-2])
+        return dp[n-1]</t>
+  </si>
+  <si>
+    <t>read O(n) space solution, then try O(1) solution</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D0A7-2B23-DB41-A123-92CA1A1D8EFD}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2492,7 +2536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -2512,7 +2556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -2535,7 +2579,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -2558,7 +2602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>131</v>
       </c>
@@ -2578,7 +2622,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>131</v>
       </c>
@@ -2601,7 +2645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -2621,7 +2665,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>162</v>
       </c>
@@ -2644,47 +2688,68 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>162</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="F40" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F42" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F44" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F46" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F48" t="s">
         <v>13</v>
       </c>
@@ -3061,6 +3126,7 @@
     <hyperlink ref="B36" r:id="rId36" display="https://neetcode.io/problems/valid-binary-search-tree" xr:uid="{03349B3C-ABAB-B94A-8A26-5E068E87E65A}"/>
     <hyperlink ref="B38" r:id="rId37" display="https://neetcode.io/problems/binary-tree-from-preorder-and-inorder-traversal" xr:uid="{C00137CB-E00D-5E42-B4F5-2278B255197B}"/>
     <hyperlink ref="B39" r:id="rId38" display="https://neetcode.io/problems/climbing-stairs" xr:uid="{37D160E0-9CAB-0444-BFB0-723DE0C53234}"/>
+    <hyperlink ref="B40" r:id="rId39" display="https://neetcode.io/problems/house-robber" xr:uid="{CEEDF22F-C940-E14C-8ED6-0F0B0E2BD726}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
house robber2 O(1) solution
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC82F097-C169-984E-A0D0-62B75FB7D716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C551FA1-2E4B-FD40-93ED-0BB9F1DF3A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27680" yWindow="2360" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="175">
   <si>
     <t>Category</t>
   </si>
@@ -1335,6 +1335,26 @@
   </si>
   <si>
     <t>read O(n) space solution, then try O(1) solution</t>
+  </si>
+  <si>
+    <t>same as house robber, we can either pick first or last element though, so calculate 2 results, 1 without first element, 1 without last element.</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def rob(self, nums: List[int]) -&gt; int:
+        def robHelper(nums):
+            rob1, rob2 = 0, 0
+            for n in nums:
+                temp = max(n + rob1, rob2)
+                rob1 = rob2
+                rob2 = temp
+            return rob2
+        if len(nums)==1:
+            return nums[0]
+        return max(robHelper(nums[1:]),robHelper(nums[:-1]))</t>
+  </si>
+  <si>
+    <t>House Robber II </t>
   </si>
 </sst>
 </file>
@@ -1774,7 +1794,7 @@
   <dimension ref="A1:S216"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2715,7 +2735,22 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>162</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3127,6 +3162,7 @@
     <hyperlink ref="B38" r:id="rId37" display="https://neetcode.io/problems/binary-tree-from-preorder-and-inorder-traversal" xr:uid="{C00137CB-E00D-5E42-B4F5-2278B255197B}"/>
     <hyperlink ref="B39" r:id="rId38" display="https://neetcode.io/problems/climbing-stairs" xr:uid="{37D160E0-9CAB-0444-BFB0-723DE0C53234}"/>
     <hyperlink ref="B40" r:id="rId39" display="https://neetcode.io/problems/house-robber" xr:uid="{CEEDF22F-C940-E14C-8ED6-0F0B0E2BD726}"/>
+    <hyperlink ref="B41" r:id="rId40" display="https://neetcode.io/problems/house-robber-ii" xr:uid="{CD001850-98D3-BC45-92E9-9145B51D7C2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
number of 1s - bit manipulation
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABCDE5F-8500-4248-8AF2-591F35335940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DC8417-90F9-D343-9B0F-3E95C1A544B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28020" yWindow="2280" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="240">
   <si>
     <t>Category</t>
   </si>
@@ -1746,6 +1746,65 @@
   </si>
   <si>
     <t>Merge Intervals </t>
+  </si>
+  <si>
+    <t>Non Overlapping Intervals </t>
+  </si>
+  <si>
+    <t>if there's an overlap pick the interval which ends early</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def eraseOverlapIntervals(self, intervals: List[List[int]]) -&gt; int:
+        intervals.sort()
+        res = 0
+        prevEnd = intervals[0][1]
+        for start, end in intervals[1:]:
+            if start &gt;= prevEnd:
+                prevEnd = end
+            else:
+                res += 1
+                prevEnd = min(end, prevEnd)
+        return res</t>
+  </si>
+  <si>
+    <t>Alien Dictionary </t>
+  </si>
+  <si>
+    <t>Advanced Graphs</t>
+  </si>
+  <si>
+    <t>topological sort</t>
+  </si>
+  <si>
+    <t>Bit Manipulation
+Bit Manipulation
+Bit Manipulation</t>
+  </si>
+  <si>
+    <t>Number of 1 Bits </t>
+  </si>
+  <si>
+    <t>Counting Bits </t>
+  </si>
+  <si>
+    <t>Reverse Bits </t>
+  </si>
+  <si>
+    <t>Missing Number </t>
+  </si>
+  <si>
+    <t>Sum of Two Integers </t>
+  </si>
+  <si>
+    <t>2 ways: ANDing every digit with 1, expecting a 0. or, Modding (%) every digit with 2.( reminder will be 1). To get next digit, we can use divide by 2, or bit shift(preferred as it is efficient on CPU)</t>
+  </si>
+  <si>
+    <t>slightly more optimal, also constant time. So no need to use this. Use optimal 2 solution. It's complicated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimal 2: Looks at every 1 (constant time - 32 operations, 32 bits are looked at so O(1)
+Number of 1 Bits </t>
   </si>
 </sst>
 </file>
@@ -2183,13 +2242,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D0A7-2B23-DB41-A123-92CA1A1D8EFD}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" style="6" customWidth="1"/>
@@ -3424,37 +3483,106 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>216</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>227</v>
+      </c>
       <c r="F54" t="s">
         <v>13</v>
       </c>
+      <c r="G54" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>239</v>
+      </c>
       <c r="F55" t="s">
         <v>13</v>
       </c>
+      <c r="G55" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="F56" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>234</v>
+      </c>
       <c r="F57" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>235</v>
+      </c>
       <c r="F58" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="F59" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>229</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C60" t="s">
+        <v>230</v>
+      </c>
       <c r="F60" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3784,6 +3912,13 @@
     <hyperlink ref="B51" r:id="rId50" display="https://neetcode.io/problems/longest-common-subsequence" xr:uid="{002246E8-3969-1F4E-AEA1-A3CA8A3DFB84}"/>
     <hyperlink ref="B52" r:id="rId51" display="https://neetcode.io/problems/insert-new-interval" xr:uid="{732EC2E2-DB8E-CF43-9D85-39B5E23A9042}"/>
     <hyperlink ref="B53" r:id="rId52" display="https://neetcode.io/problems/merge-intervals" xr:uid="{C938C9C9-8192-9043-AAFA-40955C078613}"/>
+    <hyperlink ref="B54" r:id="rId53" display="https://neetcode.io/problems/non-overlapping-intervals" xr:uid="{22823251-5EE1-F54A-BED7-B9F3C7E00ED5}"/>
+    <hyperlink ref="B60" r:id="rId54" display="https://neetcode.io/problems/foreign-dictionary" xr:uid="{9A2AE8DB-AA45-994B-BE5F-BDFCB583925E}"/>
+    <hyperlink ref="B55" r:id="rId55" display="https://neetcode.io/problems/number-of-one-bits" xr:uid="{1D8EE561-EEAF-EF45-95DA-0490AE5E1BB3}"/>
+    <hyperlink ref="B56" r:id="rId56" display="https://neetcode.io/problems/counting-bits" xr:uid="{3C8742FF-4C52-7945-A27E-DA6EB3129E16}"/>
+    <hyperlink ref="B57" r:id="rId57" display="https://neetcode.io/problems/reverse-bits" xr:uid="{E15627E1-508B-364D-83F0-F0BB90B6CCE4}"/>
+    <hyperlink ref="B58" r:id="rId58" display="https://neetcode.io/problems/missing-number" xr:uid="{853F6E34-42B7-4741-BCE3-B5694D2A70A1}"/>
+    <hyperlink ref="B59" r:id="rId59" display="https://neetcode.io/problems/sum-of-two-integers" xr:uid="{90FB29A5-55D2-804D-9747-BEBCB9B9BB52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bit manip - reverse + missing num
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DC8417-90F9-D343-9B0F-3E95C1A544B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09838718-8E57-F648-B57E-804E9AA2F010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28020" yWindow="2280" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="247">
   <si>
     <t>Category</t>
   </si>
@@ -1805,6 +1805,74 @@
   <si>
     <t xml:space="preserve">optimal 2: Looks at every 1 (constant time - 32 operations, 32 bits are looked at so O(1)
 Number of 1 Bits </t>
+  </si>
+  <si>
+    <t>loop from 0 to n and then use NumberOf1bits solution here(to find hammingweight) on I to find and append count to resultant array</t>
+  </si>
+  <si>
+    <t>besides 0, number of 1s for each is 1+dp[i-offset] where offset is the most significant bit's value(1,2,4,8,16,… etc(powers of 2)). finding most significant bit is by doing i==offset*2 and multiplying offset by 2 if condition is true
+class Solution:
+    def countBits(self, n: int) -&gt; List[int]:
+        dp = [0] * (n + 1)
+        offset = 1
+        for i in range(1, n + 1):
+            if offset * 2 == i:
+                offset = i
+            dp[i] = 1 + dp[i - offset]
+        return dp</t>
+  </si>
+  <si>
+    <t>see code</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def reverseBits(self, n: int) -&gt; int:
+        res = 0
+        for i in range(32):
+            bit = (n &gt;&gt; i) &amp; 1
+            res += (bit &lt;&lt; (31 - i))
+        return res
+This solution reverses the bits of a given 32-bit unsigned integer. Here’s a step-by-step explanation of the code:
+1. **Initialization**:
+   - `res` is initialized to `0`. This will store the result of the reversed bits.
+2. **Loop through each bit**:
+   - A loop runs from `0` to `31`, iterating over each bit position in the 32-bit integer `n`.
+3. **Extract the i-th bit**:
+   - `bit = (n &gt;&gt; i) &amp; 1`: This shifts the bits of `n` to the right by `i` positions, so that the i-th bit is now in the least significant bit (LSB) position. Then, it performs a bitwise AND with `1` to isolate the LSB, effectively extracting the i-th bit of `n`.
+4. **Set the corresponding bit in the result**:
+   - `res += (bit &lt;&lt; (31 - i))`: This shifts the extracted bit to its new position in the reversed bit order. The bit originally at position `i` in `n` should end up at position `31 - i` in `res`. The shifted bit is then added to `res`.
+5. **Return the result**:
+   - After the loop completes, `res` contains the reversed bit pattern of `n`, and it is returned as the final result.
+Here's an example to illustrate:
+**Example**:
+- Input: `n = 43261596` (binary representation: `00000010100101000001111010011100`)
+- Output: `964176192` (binary representation: `00111001011110000010100101000000`)
+**Detailed Steps**:
+1. Extract the 0-th bit of `n` and set it to the 31st position in `res`.
+2. Extract the 1st bit of `n` and set it to the 30th position in `res`.
+3. Continue this process for all 32 bits.
+4. The final value of `res` will have all bits of `n` reversed.
+This approach ensures that each bit is correctly placed in its reversed position, achieving the desired result.</t>
+  </si>
+  <si>
+    <t>see code, super intuitive solution. Read all available solutions for this problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use hashing, cross off any number we encounter and then return the remaining number
+</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def missingNumber(self, nums: List[int]) -&gt; int:
+        res = len(nums)
+        for i in range(len(nums)):
+            res += i - nums[i]
+        return res
+Alternative solution is using XORs(have to memorise or know this solution. can't really derive it on spot
+XORing numbers with itself will become 0, leaving out the one number that was missing
+class Solution:
+    def missingNumber(self, nums: List[int]) -&gt; int:
+        return reduce(lambda x,y: x ^ y, list(range(len(nums)+1)) + nums)</t>
   </si>
 </sst>
 </file>
@@ -2242,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D0A7-2B23-DB41-A123-92CA1A1D8EFD}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3532,7 +3600,19 @@
       <c r="B56" s="2" t="s">
         <v>233</v>
       </c>
+      <c r="C56" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>240</v>
+      </c>
       <c r="F56" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3543,7 +3623,16 @@
       <c r="B57" s="2" t="s">
         <v>234</v>
       </c>
+      <c r="C57" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="F57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3554,7 +3643,19 @@
       <c r="B58" s="2" t="s">
         <v>235</v>
       </c>
+      <c r="C58" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>245</v>
+      </c>
       <c r="F58" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
graphs - num of islands + clone graph
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09838718-8E57-F648-B57E-804E9AA2F010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A114AF0-D05E-CD49-A89E-5D518BA01DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28020" yWindow="2280" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="23360" windowHeight="14560" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="256">
   <si>
     <t>Category</t>
   </si>
@@ -1794,9 +1794,6 @@
     <t>Missing Number </t>
   </si>
   <si>
-    <t>Sum of Two Integers </t>
-  </si>
-  <si>
     <t>2 ways: ANDing every digit with 1, expecting a 0. or, Modding (%) every digit with 2.( reminder will be 1). To get next digit, we can use divide by 2, or bit shift(preferred as it is efficient on CPU)</t>
   </si>
   <si>
@@ -1873,6 +1870,67 @@
 class Solution:
     def missingNumber(self, nums: List[int]) -&gt; int:
         return reduce(lambda x,y: x ^ y, list(range(len(nums)+1)) + nums)</t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t>Number of Islands </t>
+  </si>
+  <si>
+    <t>do BFS and mark adjacent 1s as visited whenever you find a 1(non-visited), and then count it as an island</t>
+  </si>
+  <si>
+    <t>function numIslands(grid):
+    if grid is empty, return 0
+    initialize rows, cols, visited, and islands
+    define bfs function(r, c):
+        initialize queue
+        add (r, c) to visited and queue
+        while queue is not empty:
+            get current row, col from queue
+            for each direction (up, down, left, right):
+                calculate new row, col
+                if new row, col are in bounds, are '1', and not visited:
+                    add new row, col to queue and visited
+    for each cell in grid:
+        if cell is '1' and not visited:
+            call bfs for the cell
+            increment islands by 1
+    return islands</t>
+  </si>
+  <si>
+    <t>Clone Graph </t>
+  </si>
+  <si>
+    <t>hasmap to map oldnode to new created node and connect them using dfs</t>
+  </si>
+  <si>
+    <t>#1. Use a hashmap to track originals to their clones
+#2. Traverse the original graph, visiting each node once, for each node just clone it's value without the neighbors.
+#3. Traverse the original graph again, visiting each node once, for each node find it''s clone and set the original's neighbors clones as the clone's neighbors.
+#4. return oldToNew[node]</t>
+  </si>
+  <si>
+    <t>function cloneGraph(node):
+    if node is None:
+        return None
+    oldToNew = {}
+    function dfs(node):
+        if node in oldToNew:
+            return oldToNew[node]
+        copy = new Node(node.val)
+        oldToNew[node] = copy
+        for nei in node.neighbors:
+            copy.neighbors.append(dfs(nei))
+        return copy
+    return dfs(node)</t>
+  </si>
+  <si>
+    <t>in every cell use bfs or dfs to traverse and find if  decreasing grid coordinates</t>
+  </si>
+  <si>
+    <t>Pacific Atlantic Water Flow </t>
   </si>
 </sst>
 </file>
@@ -2308,10 +2366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D0A7-2B23-DB41-A123-92CA1A1D8EFD}">
-  <dimension ref="A1:S216"/>
+  <dimension ref="A1:S215"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="E68" sqref="E68:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3578,13 +3636,13 @@
         <v>232</v>
       </c>
       <c r="C55" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="E55" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="F55" t="s">
         <v>13</v>
@@ -3601,13 +3659,13 @@
         <v>233</v>
       </c>
       <c r="C56" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>241</v>
-      </c>
       <c r="E56" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F56" t="s">
         <v>13</v>
@@ -3624,10 +3682,10 @@
         <v>234</v>
       </c>
       <c r="C57" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>242</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="F57" t="s">
         <v>13</v>
@@ -3644,41 +3702,50 @@
         <v>235</v>
       </c>
       <c r="C58" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="F58" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>229</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C59" t="s">
+        <v>230</v>
+      </c>
+      <c r="F59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="F58" t="s">
-        <v>13</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="F59" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>229</v>
-      </c>
       <c r="B60" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C60" t="s">
-        <v>230</v>
+        <v>247</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>249</v>
       </c>
       <c r="F60" t="s">
         <v>13</v>
@@ -3688,11 +3755,44 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>252</v>
+      </c>
       <c r="F61" t="s">
         <v>13</v>
       </c>
+      <c r="G61" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>254</v>
+      </c>
       <c r="F62" t="s">
         <v>13</v>
       </c>
@@ -3827,11 +3927,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F89" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="89" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="90" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="91" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="92" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3958,7 +4054,6 @@
     <row r="213" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="214" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="215" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://leetcode.com/problems/best-time-to-buy-and-sell-stock/" xr:uid="{75EC1794-1CF8-A044-BE84-82BA083360E4}"/>
@@ -4014,12 +4109,14 @@
     <hyperlink ref="B52" r:id="rId51" display="https://neetcode.io/problems/insert-new-interval" xr:uid="{732EC2E2-DB8E-CF43-9D85-39B5E23A9042}"/>
     <hyperlink ref="B53" r:id="rId52" display="https://neetcode.io/problems/merge-intervals" xr:uid="{C938C9C9-8192-9043-AAFA-40955C078613}"/>
     <hyperlink ref="B54" r:id="rId53" display="https://neetcode.io/problems/non-overlapping-intervals" xr:uid="{22823251-5EE1-F54A-BED7-B9F3C7E00ED5}"/>
-    <hyperlink ref="B60" r:id="rId54" display="https://neetcode.io/problems/foreign-dictionary" xr:uid="{9A2AE8DB-AA45-994B-BE5F-BDFCB583925E}"/>
+    <hyperlink ref="B59" r:id="rId54" display="https://neetcode.io/problems/foreign-dictionary" xr:uid="{9A2AE8DB-AA45-994B-BE5F-BDFCB583925E}"/>
     <hyperlink ref="B55" r:id="rId55" display="https://neetcode.io/problems/number-of-one-bits" xr:uid="{1D8EE561-EEAF-EF45-95DA-0490AE5E1BB3}"/>
     <hyperlink ref="B56" r:id="rId56" display="https://neetcode.io/problems/counting-bits" xr:uid="{3C8742FF-4C52-7945-A27E-DA6EB3129E16}"/>
     <hyperlink ref="B57" r:id="rId57" display="https://neetcode.io/problems/reverse-bits" xr:uid="{E15627E1-508B-364D-83F0-F0BB90B6CCE4}"/>
     <hyperlink ref="B58" r:id="rId58" display="https://neetcode.io/problems/missing-number" xr:uid="{853F6E34-42B7-4741-BCE3-B5694D2A70A1}"/>
-    <hyperlink ref="B59" r:id="rId59" display="https://neetcode.io/problems/sum-of-two-integers" xr:uid="{90FB29A5-55D2-804D-9747-BEBCB9B9BB52}"/>
+    <hyperlink ref="B60" r:id="rId59" display="https://neetcode.io/problems/count-number-of-islands" xr:uid="{D819ED46-1AD5-374D-8BC0-EFC815256505}"/>
+    <hyperlink ref="B61" r:id="rId60" display="https://neetcode.io/problems/clone-graph" xr:uid="{B3345676-7611-3645-B596-0FCA5ADA0AEF}"/>
+    <hyperlink ref="B62" r:id="rId61" display="https://neetcode.io/problems/pacific-atlantic-water-flow" xr:uid="{DA633310-0866-3B41-A6DE-F91E07490819}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
pacific atlantic water flow-graphs
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A114AF0-D05E-CD49-A89E-5D518BA01DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7D0D4D-08A9-8B4F-86D9-ACF51E1C92C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="23360" windowHeight="14560" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="258">
   <si>
     <t>Category</t>
   </si>
@@ -1931,6 +1931,30 @@
   </si>
   <si>
     <t>Pacific Atlantic Water Flow </t>
+  </si>
+  <si>
+    <t>start with nodes adjoining pacific ocean and graph traverse to find other nodes that can reach it. Similarly for atlantic ocean. Make sure not to repeat cells though</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Function pacificAtlantic(heights):
+    Define ROWS and COLS from the dimensions of heights
+    Initialize sets pac and atl
+    Define dfs(r, c, visit, prevHeight):
+        If (r,c) is in visit OR out of bounds OR height is less than prevHeight:
+            Return
+        Add (r, c) to visit
+        Call dfs for all 4 directions (up, down, left, right)
+    For each column c from 0 to COLS-1:
+        Call dfs for the Pacific ocean (0, c)
+        Call dfs for the Atlantic ocean (ROWS-1, c)
+    For each row r from 0 to ROWS-1:
+        Call dfs for the Pacific ocean (r, 0)
+        Call dfs for the Atlantic ocean (r, COLS-1)
+    Initialize res as an empty list
+    For each cell (r, c) in the grid:
+        If (r, c) is in both pac and atl:
+            Append (r, c) to res
+    Return res</t>
   </si>
 </sst>
 </file>
@@ -2369,7 +2393,7 @@
   <dimension ref="A1:S215"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68:E69"/>
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3785,15 +3809,18 @@
         <v>255</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>13</v>
+        <v>256</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>257</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>254</v>
       </c>
       <c r="F62" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
binary search - 2d grid
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A495A1C-0B8F-7F42-B03D-86D40432AC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D67F6B-6E8F-9643-B2A3-0A752248DF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="23360" windowHeight="14560" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
+    <workbookView xWindow="23360" yWindow="1180" windowWidth="32000" windowHeight="17520" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind75" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="286">
   <si>
     <t>Category</t>
   </si>
@@ -2074,6 +2074,15 @@
   </si>
   <si>
     <t xml:space="preserve">use sliding window + counter dicts to keep track of whether all chars of t are in s. this takes O(n^2) time. We can reduce this time by just checking count of have variables vs need variables(increment have only when complete count for a particular char has been met, say 3 Bs) + check for the character we just added if it is in have/need instead of checking for every single char in t everytime we add a char to substring window. neetcode's video explains easily. </t>
+  </si>
+  <si>
+    <t>binary search</t>
+  </si>
+  <si>
+    <t>Binary Search </t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix </t>
   </si>
 </sst>
 </file>
@@ -2513,7 +2522,7 @@
   <dimension ref="A1:S215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4619,7 +4628,7 @@
   <dimension ref="A1:S215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4725,6 +4734,9 @@
       <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="M6" s="12">
+        <v>45516</v>
+      </c>
     </row>
     <row r="7" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4756,17 +4768,41 @@
       <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="12">
+        <v>45517</v>
+      </c>
     </row>
     <row r="11" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="12">
+        <v>45517</v>
+      </c>
     </row>
     <row r="12" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -4814,7 +4850,7 @@
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -4824,7 +4860,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -4834,7 +4870,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -4844,7 +4880,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -4861,8 +4897,11 @@
       <c r="F20" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M20" s="12">
+        <v>45516</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -4870,7 +4909,7 @@
       <c r="C21" s="9"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -4878,7 +4917,7 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -4888,7 +4927,7 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -4897,7 +4936,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -4907,7 +4946,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -4915,7 +4954,7 @@
       <c r="C26" s="9"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -4924,7 +4963,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -4933,7 +4972,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -4943,7 +4982,7 @@
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>129</v>
       </c>
@@ -4951,7 +4990,7 @@
       <c r="C30" s="9"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>129</v>
       </c>
@@ -4959,7 +4998,7 @@
       <c r="C31" s="9"/>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -5470,6 +5509,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="https://neetcode.io/problems/two-integer-sum-ii" xr:uid="{E20B4E99-274F-F94E-934F-B32C28ECB826}"/>
+    <hyperlink ref="B10" r:id="rId2" display="https://neetcode.io/problems/binary-search" xr:uid="{E807CEB2-E9F7-4142-BE56-6633DCA44C77}"/>
+    <hyperlink ref="B11" r:id="rId3" display="https://neetcode.io/problems/search-2d-matrix" xr:uid="{B3E8B2E1-2889-4041-B7AE-F5280BEA4EB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
binary search sheet - 2d grid
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D67F6B-6E8F-9643-B2A3-0A752248DF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6EF089-36E6-784D-9F24-3E4C24CEB182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23360" yWindow="1180" windowWidth="32000" windowHeight="17520" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
+    <workbookView xWindow="23360" yWindow="1180" windowWidth="32000" windowHeight="17520" activeTab="1" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind75" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="287">
   <si>
     <t>Category</t>
   </si>
@@ -2083,6 +2083,9 @@
   </si>
   <si>
     <t>Search a 2D Matrix </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        #first find row, then binary search in row to find num</t>
   </si>
 </sst>
 </file>
@@ -2521,7 +2524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D0A7-2B23-DB41-A123-92CA1A1D8EFD}">
   <dimension ref="A1:S215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -4627,8 +4630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51B79D9-781F-B24C-B746-F026FC84CF77}">
   <dimension ref="A1:S215"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4792,10 +4795,10 @@
         <v>285</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
diameter of tree hint
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379122B7-272B-EB43-9A04-F6DF6D1175AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6FD95B-FE87-874D-9AC8-11C61F5CD070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23360" yWindow="-1140" windowWidth="32000" windowHeight="17520" activeTab="1" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="23360" windowHeight="14560" activeTab="1" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind75" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="296">
   <si>
     <t>Category</t>
   </si>
@@ -2104,6 +2104,15 @@
   </si>
   <si>
     <t>range of 1 to max(array) will contain k. find min k using binary search. Note that whenever answer is found, it will move search just before it. So result will always be start(when it is end+1 I guess)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter of Binary Tree </t>
+  </si>
+  <si>
+    <t>traverse through tree, calculate depth of each subtree(use dp to avoid repeated calculation) and keep updating the maximum diameter. Diameter is the maximum value found</t>
+  </si>
+  <si>
+    <t>no dp</t>
   </si>
 </sst>
 </file>
@@ -4648,8 +4657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51B79D9-781F-B24C-B746-F026FC84CF77}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5038,9 +5047,24 @@
       <c r="A31" t="s">
         <v>129</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="7"/>
+      <c r="B31" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M31" s="12">
+        <v>45524</v>
+      </c>
     </row>
     <row r="32" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">

</xml_diff>

<commit_message>
level order traversal example
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954A4AB1-5E1D-1846-81DC-BBC7D3B9B23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A1AF24-A83D-B147-8F31-2871B39151BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23360" yWindow="-1140" windowWidth="32000" windowHeight="17520" activeTab="1" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="300">
   <si>
     <t>Category</t>
   </si>
@@ -2119,6 +2119,12 @@
   </si>
   <si>
     <t>traverse through tree, calculate depth of left and right subtree for each node and check if they differ by more than an absolute value of 1. if so, then not balanced. Btw, as you calc maxDepth, use dp to store them. Avoid recalculating</t>
+  </si>
+  <si>
+    <t>Binary Tree Right Side View </t>
+  </si>
+  <si>
+    <t>level order traversal, print last node of every level</t>
   </si>
 </sst>
 </file>
@@ -4664,7 +4670,7 @@
   <dimension ref="A1:S216"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L35" activeCellId="1" sqref="M32 L35"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5095,15 +5101,30 @@
         <v>45524</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>129</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M33" s="12">
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>129</v>
       </c>
@@ -5111,7 +5132,7 @@
       <c r="C34" s="9"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>129</v>
       </c>
@@ -5119,7 +5140,7 @@
       <c r="C35" s="9"/>
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>129</v>
       </c>
@@ -5129,7 +5150,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -5137,7 +5158,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>129</v>
       </c>
@@ -5147,7 +5168,7 @@
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>129</v>
       </c>
@@ -5155,7 +5176,7 @@
       <c r="C39" s="9"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>160</v>
       </c>
@@ -5163,7 +5184,7 @@
       <c r="C40" s="9"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>160</v>
       </c>
@@ -5173,7 +5194,7 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>160</v>
       </c>
@@ -5181,7 +5202,7 @@
       <c r="C42" s="9"/>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>160</v>
       </c>
@@ -5189,7 +5210,7 @@
       <c r="C43" s="9"/>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>160</v>
       </c>
@@ -5197,7 +5218,7 @@
       <c r="C44" s="9"/>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>160</v>
       </c>
@@ -5207,7 +5228,7 @@
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
     </row>
-    <row r="46" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>160</v>
       </c>
@@ -5215,7 +5236,7 @@
       <c r="C46" s="9"/>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>160</v>
       </c>
@@ -5223,7 +5244,7 @@
       <c r="C47" s="9"/>
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>160</v>
       </c>
@@ -5611,6 +5632,7 @@
     <hyperlink ref="B2" r:id="rId4" display="https://neetcode.io/problems/permutation-string" xr:uid="{29884F37-AD83-2346-ACEC-43F6F85A0517}"/>
     <hyperlink ref="B12" r:id="rId5" display="https://neetcode.io/problems/eating-bananas" xr:uid="{4049EAEF-326B-3446-ADAF-95578592609F}"/>
     <hyperlink ref="B32" r:id="rId6" display="https://neetcode.io/problems/balanced-binary-tree" xr:uid="{14AE724F-E213-4241-98C9-CFC96687A75E}"/>
+    <hyperlink ref="B33" r:id="rId7" display="https://neetcode.io/problems/binary-tree-right-side-view" xr:uid="{859D971B-2CF1-D341-B886-45F2811A9CC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
simple binary tree traversal problem
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A1AF24-A83D-B147-8F31-2871B39151BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4389D462-28AB-EA4E-B4BC-47F808BE704A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23360" yWindow="-1140" windowWidth="32000" windowHeight="17520" activeTab="1" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="302">
   <si>
     <t>Category</t>
   </si>
@@ -2125,6 +2125,12 @@
   </si>
   <si>
     <t>level order traversal, print last node of every level</t>
+  </si>
+  <si>
+    <t>Count Good Nodes In Binary Tree </t>
+  </si>
+  <si>
+    <t>simple traversal keeping track of parent value</t>
   </si>
 </sst>
 </file>
@@ -4670,7 +4676,7 @@
   <dimension ref="A1:S216"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5128,9 +5134,24 @@
       <c r="A34" t="s">
         <v>129</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="7"/>
+      <c r="B34" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="12">
+        <v>45527</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -5633,6 +5654,7 @@
     <hyperlink ref="B12" r:id="rId5" display="https://neetcode.io/problems/eating-bananas" xr:uid="{4049EAEF-326B-3446-ADAF-95578592609F}"/>
     <hyperlink ref="B32" r:id="rId6" display="https://neetcode.io/problems/balanced-binary-tree" xr:uid="{14AE724F-E213-4241-98C9-CFC96687A75E}"/>
     <hyperlink ref="B33" r:id="rId7" display="https://neetcode.io/problems/binary-tree-right-side-view" xr:uid="{859D971B-2CF1-D341-B886-45F2811A9CC0}"/>
+    <hyperlink ref="B34" r:id="rId8" display="https://neetcode.io/problems/count-good-nodes-in-binary-tree" xr:uid="{C0104A18-6E87-9F43-B17D-23ACB3EF46AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Min cost climbing stairs
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AF2F41-782B-784E-9259-6CED2D9129EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CCE080-A3C3-F54D-90D6-E422764F5C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23360" yWindow="-1140" windowWidth="32000" windowHeight="17520" activeTab="1" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="307">
   <si>
     <t>Category</t>
   </si>
@@ -2137,6 +2137,27 @@
   </si>
   <si>
     <t>traverse old linkedlist to create mapping of each node and its copies. Traverse again to replicate copies</t>
+  </si>
+  <si>
+    <t>Min Cost Climbing Stairs </t>
+  </si>
+  <si>
+    <t>climbing stairs problem+two robber problem</t>
+  </si>
+  <si>
+    <t>Imagine you’re climbing stairs where each step has a different price. To minimize the total cost, you can either take one step or two steps at a time. We calculate the cheapest way to reach the top by considering the cost of each step and choosing the least expensive option for each move.
+function minCostClimbingStairs(cost):
+    if length of cost is 0:
+        return 0
+    if length of cost is 1:
+        return cost[0]
+    initialize dp0 to cost[0]
+    initialize dp1 to cost[1]
+    for i from 2 to length of cost - 1:
+        cur = cost[i] + min(dp0, dp1)
+        update dp0 to dp1
+        update dp1 to cur
+    return min(dp0, dp1)</t>
   </si>
 </sst>
 </file>
@@ -4681,8 +4702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51B79D9-781F-B24C-B746-F026FC84CF77}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5215,14 +5236,27 @@
       <c r="B39" s="2"/>
       <c r="C39" s="9"/>
       <c r="D39" s="7"/>
+      <c r="M39" s="12"/>
     </row>
     <row r="40" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>160</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="7"/>
+      <c r="B40" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M40" s="12">
+        <v>45528</v>
+      </c>
     </row>
     <row r="41" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -5675,6 +5709,7 @@
     <hyperlink ref="B33" r:id="rId7" display="https://neetcode.io/problems/binary-tree-right-side-view" xr:uid="{859D971B-2CF1-D341-B886-45F2811A9CC0}"/>
     <hyperlink ref="B34" r:id="rId8" display="https://neetcode.io/problems/count-good-nodes-in-binary-tree" xr:uid="{C0104A18-6E87-9F43-B17D-23ACB3EF46AA}"/>
     <hyperlink ref="B13" r:id="rId9" display="https://neetcode.io/problems/copy-linked-list-with-random-pointer" xr:uid="{FE67A5B3-78B2-7347-B3AD-4344407B4BF5}"/>
+    <hyperlink ref="B40" r:id="rId10" display="https://neetcode.io/problems/min-cost-climbing-stairs" xr:uid="{8C24C7B2-1EBF-2948-99D3-ABB1C818BC91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reverse nodes in k groups
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B93AB11-1575-4041-885F-F5C47EA83D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C208BE3-E183-BB45-85E3-F8AECAED8635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="23360" windowHeight="14660" activeTab="1" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="325">
   <si>
     <t>Category</t>
   </si>
@@ -2258,6 +2258,12 @@
   </si>
   <si>
     <t>w</t>
+  </si>
+  <si>
+    <t>Reverse Nodes In K Group </t>
+  </si>
+  <si>
+    <t>have a dummy pointer to handle edge cases .find kth node, then reverse for every group and connect it to kth node's next node. And previous groups last node.</t>
   </si>
 </sst>
 </file>
@@ -4811,7 +4817,7 @@
   <dimension ref="A1:S216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5084,12 +5090,21 @@
       <c r="A16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="7"/>
+      <c r="B16" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>324</v>
+      </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="4"/>
       <c r="J16" s="11"/>
+      <c r="M16" s="12">
+        <v>45538</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -5891,6 +5906,7 @@
     <hyperlink ref="B61" r:id="rId13" display="https://neetcode.io/problems/rotting-fruit" xr:uid="{BCC70CEE-A3BE-3B41-8C6A-C77DE31A3267}"/>
     <hyperlink ref="B62" r:id="rId14" display="https://neetcode.io/problems/max-area-of-island" xr:uid="{5A62210C-BAD0-0A4A-8370-5D98AE9EB443}"/>
     <hyperlink ref="B63" r:id="rId15" display="https://neetcode.io/problems/surrounded-regions" xr:uid="{86AEEEA6-AA31-E54C-A753-BD1D2DED0599}"/>
+    <hyperlink ref="B16" r:id="rId16" display="https://neetcode.io/problems/reverse-nodes-in-k-group" xr:uid="{7923683B-D2D1-074B-8773-9FF02C2283E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
middle of ll -second node if even
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21C8E2B-330B-C043-9B7A-FC0C71D73ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D95B7D9-E65F-1341-8AB3-C2383BE6329D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -2841,7 +2841,7 @@
   <dimension ref="A1:S215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3060,7 +3060,7 @@
         <v>45510</v>
       </c>
       <c r="N6" s="12">
-        <v>45516</v>
+        <v>45580</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3237,7 +3237,9 @@
       <c r="M12" s="12">
         <v>45510</v>
       </c>
-      <c r="N12" s="12"/>
+      <c r="N12" s="12">
+        <v>45597</v>
+      </c>
     </row>
     <row r="13" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -3321,7 +3323,9 @@
       <c r="M15" s="12">
         <v>45510</v>
       </c>
-      <c r="N15" s="12"/>
+      <c r="N15" s="12">
+        <v>45597</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -3504,7 +3508,9 @@
       <c r="M22" s="12">
         <v>45510</v>
       </c>
-      <c r="N22" s="12"/>
+      <c r="N22" s="12">
+        <v>45580</v>
+      </c>
     </row>
     <row r="23" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -4947,7 +4953,7 @@
   <dimension ref="A1:S224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5236,7 +5242,7 @@
         <v>45538</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -5254,7 +5260,7 @@
         <v>45543</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -5264,7 +5270,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -5285,7 +5291,7 @@
         <v>45545</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -5304,7 +5310,7 @@
         <v>45546</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -5314,7 +5320,7 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -5324,7 +5330,7 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -5334,7 +5340,7 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -5344,7 +5350,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -5354,7 +5360,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -5364,7 +5370,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -5374,7 +5380,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -5384,7 +5390,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -5404,8 +5410,11 @@
       <c r="M29" s="12">
         <v>45516</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N29" s="12">
+        <v>45597</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -5413,7 +5422,7 @@
       <c r="C30" s="9"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -5421,7 +5430,7 @@
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
     </row>
-    <row r="32" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
find town judge - degree analysis
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472B242D-3ADC-BB45-927A-49C808BB7652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2703CC-AFE5-584C-B4F7-2323C5E74200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="23360" windowHeight="14660" activeTab="1" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="345">
   <si>
     <t>Category</t>
   </si>
@@ -2425,6 +2425,12 @@
   </si>
   <si>
     <t>2 sols: dp by going in reverse or monotonic stack</t>
+  </si>
+  <si>
+    <t>Course Schedule </t>
+  </si>
+  <si>
+    <t>tpological sort dfs in a checklist like approach</t>
   </si>
 </sst>
 </file>
@@ -4985,10 +4991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51B79D9-781F-B24C-B746-F026FC84CF77}">
-  <dimension ref="A1:S225"/>
+  <dimension ref="A1:S226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5984,40 +5990,51 @@
     </row>
     <row r="73" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="7"/>
+        <v>243</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="D73" s="9"/>
+      <c r="F73" s="4"/>
+      <c r="M73" s="12">
+        <v>45610</v>
+      </c>
     </row>
     <row r="74" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
         <v>255</v>
       </c>
       <c r="B74" s="2"/>
-      <c r="C74" s="6"/>
+      <c r="C74" s="9"/>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="7"/>
+    </row>
     <row r="76" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="78" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="79" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="80" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" spans="4:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G81" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="81" spans="4:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" spans="4:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D82" s="6" t="s">
+      <c r="G82" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="4:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D83" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="G82" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="83" spans="4:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G83" t="s">
         <v>13</v>
       </c>
@@ -6097,7 +6114,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="7:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" spans="7:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G99" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="100" spans="7:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="7:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="102" spans="7:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6224,6 +6245,7 @@
     <row r="223" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="224" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="225" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="https://neetcode.io/problems/two-integer-sum-ii" xr:uid="{E20B4E99-274F-F94E-934F-B32C28ECB826}"/>
@@ -6248,6 +6270,7 @@
     <hyperlink ref="B50" r:id="rId20" display="https://neetcode.io/problems/maximum-product-subarray" xr:uid="{4AB51B69-3378-E646-96DE-EE9099589DBC}"/>
     <hyperlink ref="B10" r:id="rId21" display="https://neetcode.io/problems/validate-parentheses" xr:uid="{891F700B-D86D-4546-907D-1E430C94BA7F}"/>
     <hyperlink ref="B9" r:id="rId22" display="https://neetcode.io/problems/daily-temperatures" xr:uid="{F6C74299-E2F9-134C-BFFC-2EC4312B37D7}"/>
+    <hyperlink ref="B73" r:id="rId23" display="https://neetcode.io/problems/course-schedule" xr:uid="{408CB3A3-BBFD-624F-ACE2-8C813CA064D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cheapest flights within k stops
</commit_message>
<xml_diff>
--- a/DSA-sheet/DSA-Sheet.xlsx
+++ b/DSA-sheet/DSA-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/DSA-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5FB1B8-64EC-7744-B2D8-0EBD5F7D8060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC0DBBF-FBB5-384E-BAD3-5C1CDD446D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="360">
   <si>
     <t>Category</t>
   </si>
@@ -2473,6 +2473,9 @@
   </si>
   <si>
     <t>manacher's algorithm</t>
+  </si>
+  <si>
+    <t>https://medium.com/@thabheloduve/here-are-one-line-solutions-for-leetcode-in-python-6e9727acc43d</t>
   </si>
 </sst>
 </file>
@@ -6323,7 +6326,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6419,6 +6422,9 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>358</v>
+      </c>
+      <c r="R9" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>